<commit_message>
Error in adding means to crosstab
</commit_message>
<xml_diff>
--- a/Tables - Nominal - Control at T1 v. T2 - weight_a.xlsx
+++ b/Tables - Nominal - Control at T1 v. T2 - weight_a.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,47 +557,47 @@
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DK/NA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>(0.0%) 0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>(0.0%) 0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Gender (P=1.000)</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Man</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>(48.8%) 394</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>(48.8%) 394</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Non-binary</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>(2.1%) 16</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>(2.1%) 16</t>
         </is>
       </c>
     </row>
@@ -605,17 +605,17 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Non-binary</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>(0.6%) 5</t>
+          <t>(2.1%) 16</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>(0.6%) 5</t>
+          <t>(2.1%) 16</t>
         </is>
       </c>
     </row>
@@ -623,7 +623,7 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Skipped</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -641,17 +641,53 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>(0.6%) 5</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>(0.6%) 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>Woman</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>(47.8%) 386</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>(47.8%) 386</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DK/NA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>(0.0%) 0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>(0.0%) 0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished ordinal. Next is ordinal report and word
</commit_message>
<xml_diff>
--- a/Tables - Nominal - Control at T1 v. T2 - weight_a.xlsx
+++ b/Tables - Nominal - Control at T1 v. T2 - weight_a.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,258 +434,272 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Group</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Control at T1 (n=745)</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Control at T2 (n=745)</t>
+          <t>Control at T1 (n = 745)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Control at T2 (n = 745)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Gender (P=1.000)</t>
-        </is>
-      </c>
+      <c r="A3" s="1" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Gender (P = 1.000)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Man</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>(48.8%) 394</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>(48.8%) 394</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
         <is>
           <t>Non-binary</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>(2.1%) 16</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>(2.1%) 16</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>(0.6%) 5</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>(0.6%) 5</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
         <is>
           <t>Skipped</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>(0.6%) 5</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>(0.6%) 5</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
         <is>
           <t>Woman</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>(47.8%) 386</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>(47.8%) 386</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
         <is>
           <t>DK/NA</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>(0.0%) 0</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>(0.0%) 0</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" s="1" t="inlineStr"/>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Interested in News (P=1.000)</t>
-        </is>
-      </c>
+      <c r="A10" s="1" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Interested in News (P = 1.000)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>Don't know</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>(7.3%) 59</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>(7.3%) 59</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
         <is>
           <t>Hardly at all</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>(9.5%) 76</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>(9.5%) 76</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
         <is>
           <t>Most of the time</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>(34.8%) 281</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>(34.8%) 281</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
         <is>
           <t>Only now and then</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>(13.9%) 112</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>(13.9%) 112</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
         <is>
           <t>Some of the time</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>(34.5%) 279</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>(34.5%) 279</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
         <is>
           <t>DK/NA</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>(0.0%) 0</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>(0.0%) 0</t>
         </is>

</xml_diff>